<commit_message>
SetCellValue DateOnly nows works. Still missing some tests
</commit_message>
<xml_diff>
--- a/2-Tests/OpenExcelSdk.Tests/10-Files/GetCellTypeAndValueDate.xlsx
+++ b/2-Tests/OpenExcelSdk.Tests/10-Files/GetCellTypeAndValueDate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a990f455bb745add/ProjetsDev/10-Pierlam/OpenExcelSdk/Dev/OpenExcelSdk/2-Tests/OpenExcelSdk.Tests/10-Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="11_AD4DB114E441178AC67DF4536695FF58683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C68F9D3-DB0A-4564-94BD-E1A89F0EC79A}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="11_AD4DB114E441178AC67DF4536695FF58683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F142818C-FB19-4D99-829A-EF130B072694}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="2475" windowWidth="16260" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10455" yWindow="3390" windowWidth="16260" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>type</t>
   </si>
@@ -40,12 +40,18 @@
   </si>
   <si>
     <t>timeOnly</t>
+  </si>
+  <si>
+    <t>dateTime, fmt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,12 +95,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -110,6 +117,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,7 +388,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -418,6 +431,14 @@
         <v>0.39925925925925926</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
+        <v>46001.524259259262</v>
+      </c>
+    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>

</xml_diff>